<commit_message>
Add spreadsheets evaluating data sources
</commit_message>
<xml_diff>
--- a/data/ons-deaths/explore/weekly_occurrences_delays.xlsx
+++ b/data/ons-deaths/explore/weekly_occurrences_delays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\covid-stats\data\ons-deaths\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE6FC2A-7CF5-4506-99AE-827DBF995F51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99A4297-7E82-4757-BCEA-43339B4E2735}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{44E385DA-E64F-4E54-B732-3ED2FD0D56D5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="2">
   <si>
     <t>Week ended</t>
   </si>
@@ -311,7 +311,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$16:$AA$16</c:f>
+              <c:f>data!$K$17:$AA$17</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -420,7 +420,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$17:$AA$17</c:f>
+              <c:f>data!$K$18:$AA$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -532,7 +532,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$18:$AA$18</c:f>
+              <c:f>data!$K$19:$AA$19</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -647,7 +647,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$19:$AA$19</c:f>
+              <c:f>data!$K$20:$AA$20</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -765,7 +765,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$20:$AA$20</c:f>
+              <c:f>data!$K$21:$AA$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -886,7 +886,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$21:$AA$21</c:f>
+              <c:f>data!$K$22:$AA$22</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1012,7 +1012,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$22:$AA$22</c:f>
+              <c:f>data!$K$23:$AA$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1141,7 +1141,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$23:$AA$23</c:f>
+              <c:f>data!$K$24:$AA$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1273,7 +1273,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$24:$AA$24</c:f>
+              <c:f>data!$K$25:$AA$25</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1408,7 +1408,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$25:$AA$25</c:f>
+              <c:f>data!$K$26:$AA$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1546,7 +1546,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$26:$AA$26</c:f>
+              <c:f>data!$K$27:$AA$27</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1687,7 +1687,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$27:$AA$27</c:f>
+              <c:f>data!$K$28:$AA$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1892,37 +1892,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2059,10 +2028,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -2113,13 +2082,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$2:$BD$2</c:f>
+              <c:f>data!$AN$3:$BD$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2201,10 +2173,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -2255,13 +2227,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$3:$BD$3</c:f>
+              <c:f>data!$AN$4:$BD$4</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2340,10 +2315,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -2394,13 +2369,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$4:$BD$4</c:f>
+              <c:f>data!$AN$5:$BD$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2473,10 +2451,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -2527,13 +2505,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$5:$BD$5</c:f>
+              <c:f>data!$AN$6:$BD$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2606,10 +2587,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -2660,13 +2641,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$6:$BD$6</c:f>
+              <c:f>data!$AN$7:$BD$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2736,10 +2720,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -2790,13 +2774,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$7:$BD$7</c:f>
+              <c:f>data!$AN$8:$BD$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2865,10 +2852,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -2919,13 +2906,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$8:$BD$8</c:f>
+              <c:f>data!$AN$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2991,10 +2981,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -3045,13 +3035,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$9:$BD$9</c:f>
+              <c:f>data!$AN$10:$BD$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -3114,10 +3107,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -3168,13 +3161,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$10:$BD$10</c:f>
+              <c:f>data!$AN$11:$BD$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -3234,10 +3230,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -3288,13 +3284,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$11:$BD$11</c:f>
+              <c:f>data!$AN$12:$BD$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -3351,10 +3350,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -3405,13 +3404,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$12:$BD$12</c:f>
+              <c:f>data!$AN$13:$BD$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -3465,10 +3467,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -3519,13 +3521,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$13:$BD$13</c:f>
+              <c:f>data!$AN$14:$BD$14</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -3577,10 +3582,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$AN$1:$BD$1</c:f>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="663"/>
                 <c:pt idx="0">
                   <c:v>44092</c:v>
                 </c:pt>
@@ -3631,13 +3636,16 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AN$14:$BD$14</c:f>
+              <c:f>data!$AN$15:$BD$15</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -3663,6 +3671,157 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-174F-4FA4-AD54-8BFF71E4167E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>data!$AN$1:$ZZ$1</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="663"/>
+                <c:pt idx="0">
+                  <c:v>44092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44106</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44127</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44134</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44141</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44148</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44155</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44162</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44169</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44176</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44183</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44190</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44211</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AN$2:$ZZ$2</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="663"/>
+                <c:pt idx="0">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1273</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1695</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2219</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3068</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2919</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3213</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3740</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4697</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5742</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6588</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A16B-4B62-909B-56403ADE7678}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3807,37 +3966,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5036,16 +5164,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5372,10 +5500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDBD85A-8CC0-4376-BED9-08DBA7D64ACF}">
-  <dimension ref="A1:CR27"/>
+  <dimension ref="A1:CR28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
@@ -5392,11 +5520,10 @@
     <col min="29" max="33" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="41" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="51" max="54" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="56" width="9" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="55" max="57" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:95" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5563,7 +5690,9 @@
       <c r="BD1" s="3">
         <v>44204</v>
       </c>
-      <c r="BE1"/>
+      <c r="BE1" s="3">
+        <v>44211</v>
+      </c>
     </row>
     <row r="2" spans="1:95" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -5604,34 +5733,34 @@
         <v>44</v>
       </c>
       <c r="N2" s="7">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="O2" s="7">
         <v>1882</v>
       </c>
       <c r="P2" s="7">
-        <v>5193</v>
+        <v>5195</v>
       </c>
       <c r="Q2" s="7">
-        <v>8264</v>
+        <v>8265</v>
       </c>
       <c r="R2" s="7">
-        <v>8332</v>
+        <v>8334</v>
       </c>
       <c r="S2" s="7">
         <v>6955</v>
       </c>
       <c r="T2" s="7">
-        <v>5228</v>
+        <v>5230</v>
       </c>
       <c r="U2" s="7">
         <v>3992</v>
       </c>
       <c r="V2" s="7">
-        <v>2868</v>
+        <v>2869</v>
       </c>
       <c r="W2" s="7">
-        <v>2291</v>
+        <v>2294</v>
       </c>
       <c r="X2" s="7">
         <v>1786</v>
@@ -5643,13 +5772,13 @@
         <v>954</v>
       </c>
       <c r="AA2" s="7">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="AB2" s="7">
         <v>590</v>
       </c>
       <c r="AC2" s="7">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AD2" s="7">
         <v>337</v>
@@ -5682,16 +5811,16 @@
         <v>101</v>
       </c>
       <c r="AN2" s="7">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AO2" s="7">
         <v>245</v>
       </c>
       <c r="AP2" s="7">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AQ2" s="7">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="AR2" s="7">
         <v>776</v>
@@ -5700,40 +5829,42 @@
         <v>1273</v>
       </c>
       <c r="AT2" s="7">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="AU2" s="7">
-        <v>2212</v>
+        <v>2219</v>
       </c>
       <c r="AV2" s="7">
-        <v>2629</v>
+        <v>2632</v>
       </c>
       <c r="AW2" s="7">
-        <v>2897</v>
+        <v>2900</v>
       </c>
       <c r="AX2" s="7">
-        <v>3061</v>
+        <v>3068</v>
       </c>
       <c r="AY2" s="7">
-        <v>2911</v>
+        <v>2919</v>
       </c>
       <c r="AZ2" s="7">
-        <v>2831</v>
+        <v>2855</v>
       </c>
       <c r="BA2" s="7">
-        <v>3199</v>
+        <v>3213</v>
       </c>
       <c r="BB2" s="7">
-        <v>3698</v>
+        <v>3740</v>
       </c>
       <c r="BC2" s="7">
-        <v>4561</v>
+        <v>4697</v>
       </c>
       <c r="BD2" s="8">
-        <v>4863</v>
-      </c>
-      <c r="BE2" s="7"/>
-      <c r="BF2" s="9"/>
+        <v>5742</v>
+      </c>
+      <c r="BE2" s="7">
+        <v>6588</v>
+      </c>
+      <c r="BF2" s="7"/>
       <c r="BG2" s="9"/>
       <c r="BH2" s="9"/>
       <c r="BI2" s="9"/>
@@ -5772,172 +5903,174 @@
       <c r="CP2" s="9"/>
       <c r="CQ2" s="9"/>
     </row>
-    <row r="3" spans="1:95" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:95" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="10">
-        <v>0</v>
-      </c>
-      <c r="D3" s="10">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10">
-        <v>0</v>
-      </c>
-      <c r="F3" s="10">
-        <v>0</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
         <v>1</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="7">
         <v>1</v>
       </c>
-      <c r="I3" s="10">
-        <v>0</v>
-      </c>
-      <c r="J3" s="10">
-        <v>0</v>
-      </c>
-      <c r="K3" s="10">
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
         <v>1</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="7">
         <v>6</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="7">
         <v>44</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="7">
         <v>406</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="7">
         <v>1882</v>
       </c>
-      <c r="P3" s="10">
-        <v>5192</v>
-      </c>
-      <c r="Q3" s="10">
-        <v>8263</v>
-      </c>
-      <c r="R3" s="10">
-        <v>8331</v>
-      </c>
-      <c r="S3" s="10">
-        <v>6954</v>
-      </c>
-      <c r="T3" s="10">
+      <c r="P3" s="7">
+        <v>5193</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>8264</v>
+      </c>
+      <c r="R3" s="7">
+        <v>8332</v>
+      </c>
+      <c r="S3" s="7">
+        <v>6955</v>
+      </c>
+      <c r="T3" s="7">
         <v>5228</v>
       </c>
-      <c r="U3" s="10">
-        <v>3991</v>
-      </c>
-      <c r="V3" s="10">
+      <c r="U3" s="7">
+        <v>3992</v>
+      </c>
+      <c r="V3" s="7">
         <v>2868</v>
       </c>
-      <c r="W3" s="10">
-        <v>2289</v>
-      </c>
-      <c r="X3" s="10">
-        <v>1785</v>
-      </c>
-      <c r="Y3" s="10">
+      <c r="W3" s="7">
+        <v>2291</v>
+      </c>
+      <c r="X3" s="7">
+        <v>1786</v>
+      </c>
+      <c r="Y3" s="7">
         <v>1314</v>
       </c>
-      <c r="Z3" s="10">
-        <v>953</v>
-      </c>
-      <c r="AA3" s="10">
-        <v>680</v>
-      </c>
-      <c r="AB3" s="10">
+      <c r="Z3" s="7">
+        <v>954</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>682</v>
+      </c>
+      <c r="AB3" s="7">
         <v>590</v>
       </c>
-      <c r="AC3" s="10">
-        <v>428</v>
-      </c>
-      <c r="AD3" s="10">
+      <c r="AC3" s="7">
+        <v>427</v>
+      </c>
+      <c r="AD3" s="7">
         <v>337</v>
       </c>
-      <c r="AE3" s="10">
+      <c r="AE3" s="7">
         <v>233</v>
       </c>
-      <c r="AF3" s="10">
+      <c r="AF3" s="7">
         <v>194</v>
       </c>
-      <c r="AG3" s="10">
-        <v>164</v>
-      </c>
-      <c r="AH3" s="10">
+      <c r="AG3" s="7">
+        <v>165</v>
+      </c>
+      <c r="AH3" s="7">
         <v>134</v>
       </c>
-      <c r="AI3" s="10">
+      <c r="AI3" s="7">
         <v>141</v>
       </c>
-      <c r="AJ3" s="10">
+      <c r="AJ3" s="7">
         <v>102</v>
       </c>
-      <c r="AK3" s="10">
+      <c r="AK3" s="7">
         <v>92</v>
       </c>
-      <c r="AL3" s="10">
+      <c r="AL3" s="7">
         <v>77</v>
       </c>
-      <c r="AM3" s="10">
+      <c r="AM3" s="7">
         <v>101</v>
       </c>
-      <c r="AN3" s="10">
+      <c r="AN3" s="7">
         <v>168</v>
       </c>
-      <c r="AO3" s="10">
+      <c r="AO3" s="7">
         <v>245</v>
       </c>
-      <c r="AP3" s="10">
-        <v>379</v>
-      </c>
-      <c r="AQ3" s="10">
-        <v>528</v>
-      </c>
-      <c r="AR3" s="10">
-        <v>774</v>
-      </c>
-      <c r="AS3" s="10">
-        <v>1272</v>
-      </c>
-      <c r="AT3" s="10">
-        <v>1693</v>
-      </c>
-      <c r="AU3" s="9">
-        <v>2208</v>
-      </c>
-      <c r="AV3" s="9">
-        <v>2624</v>
-      </c>
-      <c r="AW3" s="9">
-        <v>2878</v>
-      </c>
-      <c r="AX3" s="9">
-        <v>3040</v>
-      </c>
-      <c r="AY3" s="9">
-        <v>2901</v>
-      </c>
-      <c r="AZ3" s="9">
-        <v>2814</v>
-      </c>
-      <c r="BA3" s="9">
-        <v>3165</v>
-      </c>
-      <c r="BB3" s="9">
-        <v>3507</v>
-      </c>
-      <c r="BC3" s="9">
-        <v>3471</v>
-      </c>
-      <c r="BD3" s="9"/>
-      <c r="BE3" s="9"/>
+      <c r="AP3" s="7">
+        <v>380</v>
+      </c>
+      <c r="AQ3" s="7">
+        <v>529</v>
+      </c>
+      <c r="AR3" s="7">
+        <v>776</v>
+      </c>
+      <c r="AS3" s="7">
+        <v>1273</v>
+      </c>
+      <c r="AT3" s="7">
+        <v>1694</v>
+      </c>
+      <c r="AU3" s="7">
+        <v>2212</v>
+      </c>
+      <c r="AV3" s="7">
+        <v>2629</v>
+      </c>
+      <c r="AW3" s="7">
+        <v>2897</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>3061</v>
+      </c>
+      <c r="AY3" s="7">
+        <v>2911</v>
+      </c>
+      <c r="AZ3" s="7">
+        <v>2831</v>
+      </c>
+      <c r="BA3" s="7">
+        <v>3199</v>
+      </c>
+      <c r="BB3" s="7">
+        <v>3698</v>
+      </c>
+      <c r="BC3" s="7">
+        <v>4561</v>
+      </c>
+      <c r="BD3" s="8">
+        <v>4863</v>
+      </c>
+      <c r="BE3" s="7"/>
       <c r="BF3" s="9"/>
       <c r="BG3" s="9"/>
       <c r="BH3" s="9"/>
@@ -5975,167 +6108,172 @@
       <c r="CN3" s="9"/>
       <c r="CO3" s="9"/>
       <c r="CP3" s="9"/>
+      <c r="CQ3" s="9"/>
     </row>
     <row r="4" spans="1:95" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="10">
         <v>1</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="10">
         <v>1</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="10">
         <v>6</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="10">
         <v>44</v>
       </c>
-      <c r="N4">
-        <v>405</v>
-      </c>
-      <c r="O4">
+      <c r="N4" s="10">
+        <v>406</v>
+      </c>
+      <c r="O4" s="10">
         <v>1882</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="10">
         <v>5192</v>
       </c>
-      <c r="Q4">
-        <v>8261</v>
-      </c>
-      <c r="R4">
-        <v>8329</v>
-      </c>
-      <c r="S4">
-        <v>6950</v>
-      </c>
-      <c r="T4">
-        <v>5226</v>
-      </c>
-      <c r="U4">
+      <c r="Q4" s="10">
+        <v>8263</v>
+      </c>
+      <c r="R4" s="10">
+        <v>8331</v>
+      </c>
+      <c r="S4" s="10">
+        <v>6954</v>
+      </c>
+      <c r="T4" s="10">
+        <v>5228</v>
+      </c>
+      <c r="U4" s="10">
         <v>3991</v>
       </c>
-      <c r="V4">
-        <v>2866</v>
-      </c>
-      <c r="W4">
-        <v>2285</v>
-      </c>
-      <c r="X4">
+      <c r="V4" s="10">
+        <v>2868</v>
+      </c>
+      <c r="W4" s="10">
+        <v>2289</v>
+      </c>
+      <c r="X4" s="10">
         <v>1785</v>
       </c>
-      <c r="Y4">
-        <v>1312</v>
-      </c>
-      <c r="Z4">
-        <v>951</v>
-      </c>
-      <c r="AA4">
-        <v>679</v>
-      </c>
-      <c r="AB4">
-        <v>588</v>
-      </c>
-      <c r="AC4">
+      <c r="Y4" s="10">
+        <v>1314</v>
+      </c>
+      <c r="Z4" s="10">
+        <v>953</v>
+      </c>
+      <c r="AA4" s="10">
+        <v>680</v>
+      </c>
+      <c r="AB4" s="10">
+        <v>590</v>
+      </c>
+      <c r="AC4" s="10">
         <v>428</v>
       </c>
-      <c r="AD4">
-        <v>335</v>
-      </c>
-      <c r="AE4">
+      <c r="AD4" s="10">
+        <v>337</v>
+      </c>
+      <c r="AE4" s="10">
         <v>233</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="10">
         <v>194</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="10">
         <v>164</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="10">
         <v>134</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="10">
         <v>141</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="10">
         <v>102</v>
       </c>
-      <c r="AK4">
+      <c r="AK4" s="10">
         <v>92</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="10">
         <v>77</v>
       </c>
-      <c r="AM4">
-        <v>100</v>
-      </c>
-      <c r="AN4">
+      <c r="AM4" s="10">
+        <v>101</v>
+      </c>
+      <c r="AN4" s="10">
         <v>168</v>
       </c>
-      <c r="AO4">
+      <c r="AO4" s="10">
         <v>245</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" s="10">
         <v>379</v>
       </c>
-      <c r="AQ4">
-        <v>527</v>
-      </c>
-      <c r="AR4">
+      <c r="AQ4" s="10">
+        <v>528</v>
+      </c>
+      <c r="AR4" s="10">
         <v>774</v>
       </c>
-      <c r="AS4">
-        <v>1270</v>
-      </c>
-      <c r="AT4">
-        <v>1690</v>
-      </c>
-      <c r="AU4" s="11">
-        <v>2205</v>
-      </c>
-      <c r="AV4" s="11">
-        <v>2610</v>
-      </c>
-      <c r="AW4" s="11">
-        <v>2849</v>
+      <c r="AS4" s="10">
+        <v>1272</v>
+      </c>
+      <c r="AT4" s="10">
+        <v>1693</v>
+      </c>
+      <c r="AU4" s="9">
+        <v>2208</v>
+      </c>
+      <c r="AV4" s="9">
+        <v>2624</v>
+      </c>
+      <c r="AW4" s="9">
+        <v>2878</v>
       </c>
       <c r="AX4" s="9">
-        <v>3019</v>
+        <v>3040</v>
       </c>
       <c r="AY4" s="9">
-        <v>2885</v>
+        <v>2901</v>
       </c>
       <c r="AZ4" s="9">
-        <v>2752</v>
+        <v>2814</v>
       </c>
       <c r="BA4" s="9">
-        <v>2541</v>
-      </c>
-      <c r="BB4" s="9"/>
-      <c r="BC4" s="9"/>
+        <v>3165</v>
+      </c>
+      <c r="BB4" s="9">
+        <v>3507</v>
+      </c>
+      <c r="BC4" s="9">
+        <v>3471</v>
+      </c>
       <c r="BD4" s="9"/>
       <c r="BE4" s="9"/>
       <c r="BF4" s="9"/>
@@ -6175,7 +6313,6 @@
       <c r="CN4" s="9"/>
       <c r="CO4" s="9"/>
       <c r="CP4" s="9"/>
-      <c r="CQ4" s="9"/>
     </row>
     <row r="5" spans="1:95" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -6435,25 +6572,25 @@
         <v>6950</v>
       </c>
       <c r="T6">
-        <v>5225</v>
+        <v>5226</v>
       </c>
       <c r="U6">
-        <v>3990</v>
+        <v>3991</v>
       </c>
       <c r="V6">
-        <v>2864</v>
+        <v>2866</v>
       </c>
       <c r="W6">
         <v>2285</v>
       </c>
       <c r="X6">
-        <v>1784</v>
+        <v>1785</v>
       </c>
       <c r="Y6">
         <v>1312</v>
       </c>
       <c r="Z6">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="AA6">
         <v>679</v>
@@ -6504,36 +6641,38 @@
         <v>379</v>
       </c>
       <c r="AQ6">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="AR6">
         <v>774</v>
       </c>
       <c r="AS6">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="AT6">
-        <v>1688</v>
+        <v>1690</v>
       </c>
       <c r="AU6" s="11">
-        <v>2201</v>
+        <v>2205</v>
       </c>
       <c r="AV6" s="11">
-        <v>2603</v>
+        <v>2610</v>
       </c>
       <c r="AW6" s="11">
-        <v>2841</v>
+        <v>2849</v>
       </c>
       <c r="AX6" s="9">
-        <v>3009</v>
+        <v>3019</v>
       </c>
       <c r="AY6" s="9">
-        <v>2842</v>
+        <v>2885</v>
       </c>
       <c r="AZ6" s="9">
-        <v>2434</v>
-      </c>
-      <c r="BA6" s="9"/>
+        <v>2752</v>
+      </c>
+      <c r="BA6" s="9">
+        <v>2541</v>
+      </c>
       <c r="BB6" s="9"/>
       <c r="BC6" s="9"/>
       <c r="BD6" s="9"/>
@@ -6616,7 +6755,7 @@
         <v>44</v>
       </c>
       <c r="N7">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="O7">
         <v>1882</v>
@@ -6625,16 +6764,16 @@
         <v>5192</v>
       </c>
       <c r="Q7">
-        <v>8259</v>
+        <v>8261</v>
       </c>
       <c r="R7">
-        <v>8326</v>
+        <v>8329</v>
       </c>
       <c r="S7">
         <v>6950</v>
       </c>
       <c r="T7">
-        <v>5224</v>
+        <v>5225</v>
       </c>
       <c r="U7">
         <v>3990</v>
@@ -6646,13 +6785,13 @@
         <v>2285</v>
       </c>
       <c r="X7">
-        <v>1783</v>
+        <v>1784</v>
       </c>
       <c r="Y7">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="Z7">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="AA7">
         <v>679</v>
@@ -6661,10 +6800,10 @@
         <v>588</v>
       </c>
       <c r="AC7">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AD7">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AE7">
         <v>233</v>
@@ -6706,30 +6845,32 @@
         <v>526</v>
       </c>
       <c r="AR7">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="AS7">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="AT7">
-        <v>1683</v>
+        <v>1688</v>
       </c>
       <c r="AU7" s="11">
-        <v>2193</v>
+        <v>2201</v>
       </c>
       <c r="AV7" s="11">
-        <v>2590</v>
+        <v>2603</v>
       </c>
       <c r="AW7" s="11">
-        <v>2835</v>
+        <v>2841</v>
       </c>
       <c r="AX7" s="9">
-        <v>2971</v>
+        <v>3009</v>
       </c>
       <c r="AY7" s="9">
-        <v>2515</v>
-      </c>
-      <c r="AZ7" s="9"/>
+        <v>2842</v>
+      </c>
+      <c r="AZ7" s="9">
+        <v>2434</v>
+      </c>
       <c r="BA7" s="9"/>
       <c r="BB7" s="9"/>
       <c r="BC7" s="9"/>
@@ -6822,19 +6963,19 @@
         <v>5192</v>
       </c>
       <c r="Q8">
-        <v>8255</v>
+        <v>8259</v>
       </c>
       <c r="R8">
-        <v>8324</v>
+        <v>8326</v>
       </c>
       <c r="S8">
-        <v>6948</v>
+        <v>6950</v>
       </c>
       <c r="T8">
-        <v>5221</v>
+        <v>5224</v>
       </c>
       <c r="U8">
-        <v>3989</v>
+        <v>3990</v>
       </c>
       <c r="V8">
         <v>2864</v>
@@ -6843,13 +6984,13 @@
         <v>2285</v>
       </c>
       <c r="X8">
-        <v>1782</v>
+        <v>1783</v>
       </c>
       <c r="Y8">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="Z8">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="AA8">
         <v>679</v>
@@ -6858,7 +6999,7 @@
         <v>588</v>
       </c>
       <c r="AC8">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AD8">
         <v>336</v>
@@ -6879,7 +7020,7 @@
         <v>141</v>
       </c>
       <c r="AJ8">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK8">
         <v>92</v>
@@ -6897,33 +7038,35 @@
         <v>245</v>
       </c>
       <c r="AP8">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AQ8">
         <v>526</v>
       </c>
       <c r="AR8">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="AS8">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="AT8">
-        <v>1678</v>
+        <v>1683</v>
       </c>
       <c r="AU8" s="11">
-        <v>2187</v>
+        <v>2193</v>
       </c>
       <c r="AV8" s="11">
-        <v>2584</v>
+        <v>2590</v>
       </c>
       <c r="AW8" s="11">
-        <v>2808</v>
+        <v>2835</v>
       </c>
       <c r="AX8" s="9">
-        <v>2713</v>
-      </c>
-      <c r="AY8" s="9"/>
+        <v>2971</v>
+      </c>
+      <c r="AY8" s="9">
+        <v>2515</v>
+      </c>
       <c r="AZ8" s="9"/>
       <c r="BA8" s="9"/>
       <c r="BB8" s="9"/>
@@ -7014,31 +7157,31 @@
         <v>1882</v>
       </c>
       <c r="P9">
-        <v>5190</v>
+        <v>5192</v>
       </c>
       <c r="Q9">
-        <v>8252</v>
+        <v>8255</v>
       </c>
       <c r="R9">
-        <v>8322</v>
+        <v>8324</v>
       </c>
       <c r="S9">
-        <v>6946</v>
+        <v>6948</v>
       </c>
       <c r="T9">
-        <v>5219</v>
+        <v>5221</v>
       </c>
       <c r="U9">
         <v>3989</v>
       </c>
       <c r="V9">
-        <v>2862</v>
+        <v>2864</v>
       </c>
       <c r="W9">
-        <v>2284</v>
+        <v>2285</v>
       </c>
       <c r="X9">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="Y9">
         <v>1310</v>
@@ -7047,13 +7190,13 @@
         <v>950</v>
       </c>
       <c r="AA9">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="AB9">
         <v>588</v>
       </c>
       <c r="AC9">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AD9">
         <v>336</v>
@@ -7062,16 +7205,16 @@
         <v>233</v>
       </c>
       <c r="AF9">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AG9">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AH9">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AI9">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AJ9">
         <v>101</v>
@@ -7089,7 +7232,7 @@
         <v>168</v>
       </c>
       <c r="AO9">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AP9">
         <v>378</v>
@@ -7098,24 +7241,26 @@
         <v>526</v>
       </c>
       <c r="AR9">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="AS9">
-        <v>1263</v>
+        <v>1266</v>
       </c>
       <c r="AT9">
-        <v>1665</v>
+        <v>1678</v>
       </c>
       <c r="AU9" s="11">
-        <v>2179</v>
+        <v>2187</v>
       </c>
       <c r="AV9" s="11">
-        <v>2563</v>
+        <v>2584</v>
       </c>
       <c r="AW9" s="11">
-        <v>2549</v>
-      </c>
-      <c r="AX9" s="9"/>
+        <v>2808</v>
+      </c>
+      <c r="AX9" s="9">
+        <v>2713</v>
+      </c>
       <c r="AY9" s="9"/>
       <c r="AZ9" s="9"/>
       <c r="BA9" s="9"/>
@@ -7204,22 +7349,22 @@
         <v>404</v>
       </c>
       <c r="O10">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="P10">
-        <v>5189</v>
+        <v>5190</v>
       </c>
       <c r="Q10">
-        <v>8251</v>
+        <v>8252</v>
       </c>
       <c r="R10">
-        <v>8320</v>
+        <v>8322</v>
       </c>
       <c r="S10">
-        <v>6942</v>
+        <v>6946</v>
       </c>
       <c r="T10">
-        <v>5218</v>
+        <v>5219</v>
       </c>
       <c r="U10">
         <v>3989</v>
@@ -7255,13 +7400,13 @@
         <v>233</v>
       </c>
       <c r="AF10">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AG10">
         <v>163</v>
       </c>
       <c r="AH10">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AI10">
         <v>140</v>
@@ -7273,7 +7418,7 @@
         <v>92</v>
       </c>
       <c r="AL10">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AM10">
         <v>100</v>
@@ -7288,24 +7433,26 @@
         <v>378</v>
       </c>
       <c r="AQ10">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AR10">
         <v>768</v>
       </c>
       <c r="AS10">
-        <v>1258</v>
+        <v>1263</v>
       </c>
       <c r="AT10">
-        <v>1657</v>
-      </c>
-      <c r="AU10" s="9">
-        <v>2155</v>
-      </c>
-      <c r="AV10" s="9">
-        <v>2319</v>
-      </c>
-      <c r="AW10" s="9"/>
+        <v>1665</v>
+      </c>
+      <c r="AU10" s="11">
+        <v>2179</v>
+      </c>
+      <c r="AV10" s="11">
+        <v>2563</v>
+      </c>
+      <c r="AW10" s="11">
+        <v>2549</v>
+      </c>
       <c r="AX10" s="9"/>
       <c r="AY10" s="9"/>
       <c r="AZ10" s="9"/>
@@ -7398,28 +7545,28 @@
         <v>1881</v>
       </c>
       <c r="P11">
-        <v>5188</v>
+        <v>5189</v>
       </c>
       <c r="Q11">
-        <v>8249</v>
+        <v>8251</v>
       </c>
       <c r="R11">
-        <v>8317</v>
+        <v>8320</v>
       </c>
       <c r="S11">
-        <v>6940</v>
+        <v>6942</v>
       </c>
       <c r="T11">
-        <v>5214</v>
+        <v>5218</v>
       </c>
       <c r="U11">
-        <v>3986</v>
+        <v>3989</v>
       </c>
       <c r="V11">
         <v>2862</v>
       </c>
       <c r="W11">
-        <v>2283</v>
+        <v>2284</v>
       </c>
       <c r="X11">
         <v>1781</v>
@@ -7431,7 +7578,7 @@
         <v>950</v>
       </c>
       <c r="AA11">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="AB11">
         <v>588</v>
@@ -7443,7 +7590,7 @@
         <v>336</v>
       </c>
       <c r="AE11">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AF11">
         <v>192</v>
@@ -7473,27 +7620,29 @@
         <v>168</v>
       </c>
       <c r="AO11">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AP11">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AQ11">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="AR11">
-        <v>761</v>
+        <v>768</v>
       </c>
       <c r="AS11">
-        <v>1254</v>
+        <v>1258</v>
       </c>
       <c r="AT11">
-        <v>1627</v>
+        <v>1657</v>
       </c>
       <c r="AU11" s="9">
-        <v>1925</v>
-      </c>
-      <c r="AV11" s="9"/>
+        <v>2155</v>
+      </c>
+      <c r="AV11" s="9">
+        <v>2319</v>
+      </c>
       <c r="AW11" s="9"/>
       <c r="AX11" s="9"/>
       <c r="AY11" s="9"/>
@@ -7584,46 +7733,46 @@
         <v>404</v>
       </c>
       <c r="O12">
-        <v>1880</v>
+        <v>1881</v>
       </c>
       <c r="P12">
-        <v>5189</v>
+        <v>5188</v>
       </c>
       <c r="Q12">
-        <v>8245</v>
+        <v>8249</v>
       </c>
       <c r="R12">
-        <v>8316</v>
+        <v>8317</v>
       </c>
       <c r="S12">
-        <v>6939</v>
+        <v>6940</v>
       </c>
       <c r="T12">
-        <v>5213</v>
+        <v>5214</v>
       </c>
       <c r="U12">
-        <v>3984</v>
+        <v>3986</v>
       </c>
       <c r="V12">
         <v>2862</v>
       </c>
       <c r="W12">
-        <v>2282</v>
+        <v>2283</v>
       </c>
       <c r="X12">
-        <v>1780</v>
+        <v>1781</v>
       </c>
       <c r="Y12">
         <v>1310</v>
       </c>
       <c r="Z12">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="AA12">
         <v>676</v>
       </c>
       <c r="AB12">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="AC12">
         <v>425</v>
@@ -7638,13 +7787,13 @@
         <v>192</v>
       </c>
       <c r="AG12">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AH12">
         <v>132</v>
       </c>
       <c r="AI12">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AJ12">
         <v>101</v>
@@ -7665,21 +7814,23 @@
         <v>243</v>
       </c>
       <c r="AP12">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AQ12">
         <v>523</v>
       </c>
       <c r="AR12">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="AS12">
-        <v>1244</v>
+        <v>1254</v>
       </c>
       <c r="AT12">
-        <v>1443</v>
-      </c>
-      <c r="AU12" s="9"/>
+        <v>1627</v>
+      </c>
+      <c r="AU12" s="9">
+        <v>1925</v>
+      </c>
       <c r="AV12" s="9"/>
       <c r="AW12" s="9"/>
       <c r="AX12" s="9"/>
@@ -7729,141 +7880,143 @@
       <c r="CP12" s="9"/>
       <c r="CQ12" s="9"/>
     </row>
-    <row r="13" spans="1:95" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:95" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="12">
-        <v>0</v>
-      </c>
-      <c r="D13" s="13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="13">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" s="13">
-        <v>0</v>
-      </c>
-      <c r="J13" s="13">
-        <v>0</v>
-      </c>
-      <c r="K13" s="13">
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>1</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13">
         <v>6</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13">
         <v>44</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13">
         <v>404</v>
       </c>
-      <c r="O13" s="13">
+      <c r="O13">
         <v>1880</v>
       </c>
-      <c r="P13" s="13">
-        <v>5188</v>
-      </c>
-      <c r="Q13" s="9">
-        <v>8241</v>
-      </c>
-      <c r="R13" s="9">
+      <c r="P13">
+        <v>5189</v>
+      </c>
+      <c r="Q13">
+        <v>8245</v>
+      </c>
+      <c r="R13">
         <v>8316</v>
       </c>
-      <c r="S13" s="9">
-        <v>6938</v>
-      </c>
-      <c r="T13" s="9">
-        <v>5212</v>
-      </c>
-      <c r="U13" s="9">
+      <c r="S13">
+        <v>6939</v>
+      </c>
+      <c r="T13">
+        <v>5213</v>
+      </c>
+      <c r="U13">
         <v>3984</v>
       </c>
-      <c r="V13" s="9">
+      <c r="V13">
         <v>2862</v>
       </c>
-      <c r="W13" s="9">
-        <v>2281</v>
-      </c>
-      <c r="X13" s="9">
-        <v>1779</v>
-      </c>
-      <c r="Y13" s="9">
+      <c r="W13">
+        <v>2282</v>
+      </c>
+      <c r="X13">
+        <v>1780</v>
+      </c>
+      <c r="Y13">
         <v>1310</v>
       </c>
-      <c r="Z13" s="9">
+      <c r="Z13">
         <v>949</v>
       </c>
-      <c r="AA13" s="9">
+      <c r="AA13">
         <v>676</v>
       </c>
-      <c r="AB13" s="9">
+      <c r="AB13">
         <v>587</v>
       </c>
-      <c r="AC13" s="9">
+      <c r="AC13">
         <v>425</v>
       </c>
-      <c r="AD13" s="9">
+      <c r="AD13">
         <v>336</v>
       </c>
-      <c r="AE13" s="9">
+      <c r="AE13">
         <v>232</v>
       </c>
-      <c r="AF13" s="9">
+      <c r="AF13">
         <v>192</v>
       </c>
-      <c r="AG13" s="9">
+      <c r="AG13">
         <v>162</v>
       </c>
-      <c r="AH13" s="9">
+      <c r="AH13">
         <v>132</v>
       </c>
-      <c r="AI13" s="9">
-        <v>140</v>
-      </c>
-      <c r="AJ13" s="9">
+      <c r="AI13">
+        <v>139</v>
+      </c>
+      <c r="AJ13">
         <v>101</v>
       </c>
-      <c r="AK13" s="9">
+      <c r="AK13">
         <v>92</v>
       </c>
-      <c r="AL13" s="9">
+      <c r="AL13">
         <v>76</v>
       </c>
-      <c r="AM13" s="9">
-        <v>99</v>
-      </c>
-      <c r="AN13" s="9">
-        <v>167</v>
-      </c>
-      <c r="AO13" s="9">
-        <v>242</v>
-      </c>
-      <c r="AP13" s="9">
-        <v>373</v>
-      </c>
-      <c r="AQ13" s="9">
-        <v>520</v>
-      </c>
-      <c r="AR13" s="9">
-        <v>750</v>
-      </c>
-      <c r="AS13" s="9">
-        <v>1097</v>
-      </c>
-      <c r="AT13" s="9"/>
+      <c r="AM13">
+        <v>100</v>
+      </c>
+      <c r="AN13">
+        <v>168</v>
+      </c>
+      <c r="AO13">
+        <v>243</v>
+      </c>
+      <c r="AP13">
+        <v>376</v>
+      </c>
+      <c r="AQ13">
+        <v>523</v>
+      </c>
+      <c r="AR13">
+        <v>755</v>
+      </c>
+      <c r="AS13">
+        <v>1244</v>
+      </c>
+      <c r="AT13">
+        <v>1443</v>
+      </c>
       <c r="AU13" s="9"/>
       <c r="AV13" s="9"/>
       <c r="AW13" s="9"/>
@@ -7953,37 +8106,37 @@
         <v>44</v>
       </c>
       <c r="N14" s="13">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="O14" s="13">
         <v>1880</v>
       </c>
       <c r="P14" s="13">
-        <v>5187</v>
+        <v>5188</v>
       </c>
       <c r="Q14" s="9">
-        <v>8240</v>
+        <v>8241</v>
       </c>
       <c r="R14" s="9">
-        <v>8315</v>
+        <v>8316</v>
       </c>
       <c r="S14" s="9">
-        <v>6937</v>
+        <v>6938</v>
       </c>
       <c r="T14" s="9">
-        <v>5210</v>
+        <v>5212</v>
       </c>
       <c r="U14" s="9">
-        <v>3982</v>
+        <v>3984</v>
       </c>
       <c r="V14" s="9">
-        <v>2860</v>
+        <v>2862</v>
       </c>
       <c r="W14" s="9">
         <v>2281</v>
       </c>
       <c r="X14" s="9">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="Y14" s="9">
         <v>1310</v>
@@ -8022,10 +8175,10 @@
         <v>101</v>
       </c>
       <c r="AK14" s="9">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AL14" s="9">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AM14" s="9">
         <v>99</v>
@@ -8034,18 +8187,20 @@
         <v>167</v>
       </c>
       <c r="AO14" s="9">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AP14" s="9">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="AQ14" s="9">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="AR14" s="9">
-        <v>684</v>
-      </c>
-      <c r="AS14" s="9"/>
+        <v>750</v>
+      </c>
+      <c r="AS14" s="9">
+        <v>1097</v>
+      </c>
       <c r="AT14" s="9"/>
       <c r="AU14" s="9"/>
       <c r="AV14" s="9"/>
@@ -8097,53 +8252,188 @@
       <c r="CP14" s="9"/>
       <c r="CQ14" s="9"/>
     </row>
-    <row r="16" spans="1:95" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="15" spans="1:95" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="12">
-        <v>0</v>
-      </c>
-      <c r="D16" s="13">
-        <v>0</v>
-      </c>
-      <c r="E16" s="13">
-        <v>0</v>
-      </c>
-      <c r="F16" s="13">
-        <v>0</v>
-      </c>
-      <c r="G16" s="13">
-        <v>0</v>
-      </c>
-      <c r="H16" s="13">
-        <v>0</v>
-      </c>
-      <c r="I16" s="13">
-        <v>0</v>
-      </c>
-      <c r="J16" s="13">
-        <v>0</v>
-      </c>
-      <c r="K16" s="13">
-        <v>0</v>
-      </c>
-      <c r="L16" s="13">
-        <v>4</v>
-      </c>
-      <c r="M16" s="13">
-        <v>35</v>
-      </c>
-      <c r="N16" s="13">
-        <v>374</v>
-      </c>
-      <c r="O16" s="13">
-        <v>1704</v>
-      </c>
-      <c r="P16" s="13">
-        <v>4117</v>
-      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="12">
+        <v>0</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13">
+        <v>1</v>
+      </c>
+      <c r="I15" s="13">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="13">
+        <v>1</v>
+      </c>
+      <c r="L15" s="13">
+        <v>6</v>
+      </c>
+      <c r="M15" s="13">
+        <v>44</v>
+      </c>
+      <c r="N15" s="13">
+        <v>405</v>
+      </c>
+      <c r="O15" s="13">
+        <v>1880</v>
+      </c>
+      <c r="P15" s="13">
+        <v>5187</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>8240</v>
+      </c>
+      <c r="R15" s="9">
+        <v>8315</v>
+      </c>
+      <c r="S15" s="9">
+        <v>6937</v>
+      </c>
+      <c r="T15" s="9">
+        <v>5210</v>
+      </c>
+      <c r="U15" s="9">
+        <v>3982</v>
+      </c>
+      <c r="V15" s="9">
+        <v>2860</v>
+      </c>
+      <c r="W15" s="9">
+        <v>2281</v>
+      </c>
+      <c r="X15" s="9">
+        <v>1778</v>
+      </c>
+      <c r="Y15" s="9">
+        <v>1310</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>949</v>
+      </c>
+      <c r="AA15" s="9">
+        <v>676</v>
+      </c>
+      <c r="AB15" s="9">
+        <v>587</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>425</v>
+      </c>
+      <c r="AD15" s="9">
+        <v>336</v>
+      </c>
+      <c r="AE15" s="9">
+        <v>232</v>
+      </c>
+      <c r="AF15" s="9">
+        <v>192</v>
+      </c>
+      <c r="AG15" s="9">
+        <v>162</v>
+      </c>
+      <c r="AH15" s="9">
+        <v>132</v>
+      </c>
+      <c r="AI15" s="9">
+        <v>140</v>
+      </c>
+      <c r="AJ15" s="9">
+        <v>101</v>
+      </c>
+      <c r="AK15" s="9">
+        <v>91</v>
+      </c>
+      <c r="AL15" s="9">
+        <v>75</v>
+      </c>
+      <c r="AM15" s="9">
+        <v>99</v>
+      </c>
+      <c r="AN15" s="9">
+        <v>167</v>
+      </c>
+      <c r="AO15" s="9">
+        <v>240</v>
+      </c>
+      <c r="AP15" s="9">
+        <v>370</v>
+      </c>
+      <c r="AQ15" s="9">
+        <v>513</v>
+      </c>
+      <c r="AR15" s="9">
+        <v>684</v>
+      </c>
+      <c r="AS15" s="9"/>
+      <c r="AT15" s="9"/>
+      <c r="AU15" s="9"/>
+      <c r="AV15" s="9"/>
+      <c r="AW15" s="9"/>
+      <c r="AX15" s="9"/>
+      <c r="AY15" s="9"/>
+      <c r="AZ15" s="9"/>
+      <c r="BA15" s="9"/>
+      <c r="BB15" s="9"/>
+      <c r="BC15" s="9"/>
+      <c r="BD15" s="9"/>
+      <c r="BE15" s="9"/>
+      <c r="BF15" s="9"/>
+      <c r="BG15" s="9"/>
+      <c r="BH15" s="9"/>
+      <c r="BI15" s="9"/>
+      <c r="BJ15" s="9"/>
+      <c r="BK15" s="9"/>
+      <c r="BL15" s="9"/>
+      <c r="BM15" s="9"/>
+      <c r="BN15" s="9"/>
+      <c r="BO15" s="9"/>
+      <c r="BP15" s="9"/>
+      <c r="BQ15" s="9"/>
+      <c r="BR15" s="9"/>
+      <c r="BS15" s="9"/>
+      <c r="BT15" s="9"/>
+      <c r="BU15" s="9"/>
+      <c r="BV15" s="9"/>
+      <c r="BW15" s="9"/>
+      <c r="BX15" s="9"/>
+      <c r="BY15" s="9"/>
+      <c r="BZ15" s="9"/>
+      <c r="CA15" s="9"/>
+      <c r="CB15" s="9"/>
+      <c r="CC15" s="9"/>
+      <c r="CD15" s="9"/>
+      <c r="CE15" s="9"/>
+      <c r="CF15" s="9"/>
+      <c r="CG15" s="9"/>
+      <c r="CH15" s="9"/>
+      <c r="CI15" s="9"/>
+      <c r="CJ15" s="9"/>
+      <c r="CK15" s="9"/>
+      <c r="CL15" s="9"/>
+      <c r="CM15" s="9"/>
+      <c r="CN15" s="9"/>
+      <c r="CO15" s="9"/>
+      <c r="CP15" s="9"/>
+      <c r="CQ15" s="9"/>
     </row>
     <row r="17" spans="1:96" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -8178,22 +8468,19 @@
         <v>0</v>
       </c>
       <c r="L17" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M17" s="13">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N17" s="13">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="O17" s="13">
-        <v>1774</v>
+        <v>1704</v>
       </c>
       <c r="P17" s="13">
-        <v>4777</v>
-      </c>
-      <c r="Q17" s="9">
-        <v>6146</v>
+        <v>4117</v>
       </c>
     </row>
     <row r="18" spans="1:96" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -8229,27 +8516,23 @@
         <v>0</v>
       </c>
       <c r="L18" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M18" s="13">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N18" s="13">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="O18" s="13">
-        <v>1806</v>
+        <v>1774</v>
       </c>
       <c r="P18" s="13">
-        <v>4989</v>
+        <v>4777</v>
       </c>
       <c r="Q18" s="9">
-        <v>7833</v>
-      </c>
-      <c r="R18" s="9">
-        <v>7288</v>
-      </c>
-      <c r="S18" s="9"/>
+        <v>6146</v>
+      </c>
     </row>
     <row r="19" spans="1:96" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -8284,32 +8567,29 @@
         <v>0</v>
       </c>
       <c r="L19" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19" s="13">
         <v>40</v>
       </c>
       <c r="N19" s="13">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="O19" s="13">
-        <v>1826</v>
+        <v>1806</v>
       </c>
       <c r="P19" s="13">
-        <v>5052</v>
+        <v>4989</v>
       </c>
       <c r="Q19" s="9">
-        <v>8013</v>
+        <v>7833</v>
       </c>
       <c r="R19" s="9">
-        <v>8036</v>
-      </c>
-      <c r="S19" s="9">
-        <v>6342</v>
-      </c>
-      <c r="T19" s="9"/>
+        <v>7288</v>
+      </c>
+      <c r="S19" s="9"/>
     </row>
-    <row r="20" spans="1:96" s="4" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:96" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
@@ -8342,33 +8622,30 @@
         <v>0</v>
       </c>
       <c r="L20" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M20" s="13">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N20" s="13">
         <v>397</v>
       </c>
       <c r="O20" s="13">
-        <v>1838</v>
+        <v>1826</v>
       </c>
       <c r="P20" s="13">
-        <v>5079</v>
+        <v>5052</v>
       </c>
       <c r="Q20" s="9">
-        <v>8073</v>
+        <v>8013</v>
       </c>
       <c r="R20" s="9">
-        <v>8121</v>
+        <v>8036</v>
       </c>
       <c r="S20" s="9">
-        <v>6746</v>
-      </c>
-      <c r="T20" s="9">
-        <v>4744</v>
-      </c>
-      <c r="U20" s="9"/>
+        <v>6342</v>
+      </c>
+      <c r="T20" s="9"/>
     </row>
     <row r="21" spans="1:96" s="4" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -8412,100 +8689,24 @@
         <v>397</v>
       </c>
       <c r="O21" s="13">
-        <v>1851</v>
+        <v>1838</v>
       </c>
       <c r="P21" s="13">
-        <v>5109</v>
+        <v>5079</v>
       </c>
       <c r="Q21" s="9">
-        <v>8104</v>
+        <v>8073</v>
       </c>
       <c r="R21" s="9">
-        <v>8152</v>
+        <v>8121</v>
       </c>
       <c r="S21" s="9">
-        <v>6790</v>
+        <v>6746</v>
       </c>
       <c r="T21" s="9">
-        <v>5048</v>
-      </c>
-      <c r="U21" s="9">
-        <v>3574</v>
-      </c>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
-      <c r="AI21" s="9"/>
-      <c r="AJ21" s="9"/>
-      <c r="AK21" s="9"/>
-      <c r="AL21" s="9"/>
-      <c r="AM21" s="9"/>
-      <c r="AN21" s="9"/>
-      <c r="AO21" s="9"/>
-      <c r="AP21" s="9"/>
-      <c r="AQ21" s="9"/>
-      <c r="AR21" s="9"/>
-      <c r="AS21" s="9"/>
-      <c r="AT21" s="9"/>
-      <c r="AU21" s="9"/>
-      <c r="AV21" s="9"/>
-      <c r="AW21" s="9"/>
-      <c r="AX21" s="9"/>
-      <c r="AY21" s="9"/>
-      <c r="AZ21" s="9"/>
-      <c r="BA21" s="9"/>
-      <c r="BB21" s="9"/>
-      <c r="BC21" s="9"/>
-      <c r="BD21" s="9"/>
-      <c r="BE21" s="9"/>
-      <c r="BF21" s="9"/>
-      <c r="BG21" s="9"/>
-      <c r="BH21" s="9"/>
-      <c r="BI21" s="9"/>
-      <c r="BJ21" s="9"/>
-      <c r="BK21" s="9"/>
-      <c r="BL21" s="9"/>
-      <c r="BM21" s="9"/>
-      <c r="BN21" s="9"/>
-      <c r="BO21" s="9"/>
-      <c r="BP21" s="9"/>
-      <c r="BQ21" s="9"/>
-      <c r="BR21" s="9"/>
-      <c r="BS21" s="9"/>
-      <c r="BT21" s="9"/>
-      <c r="BU21" s="9"/>
-      <c r="BV21" s="9"/>
-      <c r="BW21" s="9"/>
-      <c r="BX21" s="9"/>
-      <c r="BY21" s="9"/>
-      <c r="BZ21" s="9"/>
-      <c r="CA21" s="9"/>
-      <c r="CB21" s="9"/>
-      <c r="CC21" s="9"/>
-      <c r="CD21" s="9"/>
-      <c r="CE21" s="9"/>
-      <c r="CF21" s="9"/>
-      <c r="CG21" s="9"/>
-      <c r="CH21" s="9"/>
-      <c r="CI21" s="9"/>
-      <c r="CJ21" s="9"/>
-      <c r="CK21" s="9"/>
-      <c r="CL21" s="9"/>
-      <c r="CM21" s="9"/>
-      <c r="CN21" s="9"/>
-      <c r="CO21" s="9"/>
-      <c r="CP21" s="9"/>
-      <c r="CQ21" s="9"/>
+        <v>4744</v>
+      </c>
+      <c r="U21" s="9"/>
     </row>
     <row r="22" spans="1:96" s="4" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -8531,7 +8732,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="13">
         <v>0</v>
@@ -8546,32 +8747,30 @@
         <v>41</v>
       </c>
       <c r="N22" s="13">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="O22" s="13">
-        <v>1854</v>
+        <v>1851</v>
       </c>
       <c r="P22" s="13">
-        <v>5126</v>
+        <v>5109</v>
       </c>
       <c r="Q22" s="9">
-        <v>8128</v>
+        <v>8104</v>
       </c>
       <c r="R22" s="9">
-        <v>8180</v>
+        <v>8152</v>
       </c>
       <c r="S22" s="9">
-        <v>6817</v>
+        <v>6790</v>
       </c>
       <c r="T22" s="9">
-        <v>5109</v>
+        <v>5048</v>
       </c>
       <c r="U22" s="9">
-        <v>3874</v>
-      </c>
-      <c r="V22" s="9">
-        <v>2639</v>
-      </c>
+        <v>3574</v>
+      </c>
+      <c r="V22" s="9"/>
       <c r="W22" s="9"/>
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
@@ -8645,9 +8844,8 @@
       <c r="CO22" s="9"/>
       <c r="CP22" s="9"/>
       <c r="CQ22" s="9"/>
-      <c r="CR22" s="9"/>
     </row>
-    <row r="23" spans="1:96" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:96" s="4" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>1</v>
       </c>
@@ -8689,32 +8887,30 @@
         <v>399</v>
       </c>
       <c r="O23" s="13">
-        <v>1858</v>
+        <v>1854</v>
       </c>
       <c r="P23" s="13">
-        <v>5133</v>
+        <v>5126</v>
       </c>
       <c r="Q23" s="9">
-        <v>8151</v>
+        <v>8128</v>
       </c>
       <c r="R23" s="9">
-        <v>8207</v>
+        <v>8180</v>
       </c>
       <c r="S23" s="9">
-        <v>6835</v>
+        <v>6817</v>
       </c>
       <c r="T23" s="9">
-        <v>5123</v>
+        <v>5109</v>
       </c>
       <c r="U23" s="9">
-        <v>3899</v>
+        <v>3874</v>
       </c>
       <c r="V23" s="9">
-        <v>2766</v>
-      </c>
-      <c r="W23" s="9">
-        <v>1983</v>
-      </c>
+        <v>2639</v>
+      </c>
+      <c r="W23" s="9"/>
       <c r="X23" s="9"/>
       <c r="Y23" s="9"/>
       <c r="Z23" s="9"/>
@@ -8787,6 +8983,7 @@
       <c r="CO23" s="9"/>
       <c r="CP23" s="9"/>
       <c r="CQ23" s="9"/>
+      <c r="CR23" s="9"/>
     </row>
     <row r="24" spans="1:96" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
@@ -8812,7 +9009,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="13">
         <v>0</v>
@@ -8821,7 +9018,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M24" s="13">
         <v>41</v>
@@ -8830,35 +9027,33 @@
         <v>399</v>
       </c>
       <c r="O24" s="13">
-        <v>1861</v>
+        <v>1858</v>
       </c>
       <c r="P24" s="13">
-        <v>5149</v>
+        <v>5133</v>
       </c>
       <c r="Q24" s="9">
-        <v>8172</v>
+        <v>8151</v>
       </c>
       <c r="R24" s="9">
-        <v>8239</v>
+        <v>8207</v>
       </c>
       <c r="S24" s="9">
-        <v>6870</v>
+        <v>6835</v>
       </c>
       <c r="T24" s="9">
-        <v>5139</v>
+        <v>5123</v>
       </c>
       <c r="U24" s="9">
-        <v>3911</v>
+        <v>3899</v>
       </c>
       <c r="V24" s="9">
-        <v>2801</v>
+        <v>2766</v>
       </c>
       <c r="W24" s="9">
-        <v>2206</v>
-      </c>
-      <c r="X24" s="9">
-        <v>1627</v>
-      </c>
+        <v>1983</v>
+      </c>
+      <c r="X24" s="9"/>
       <c r="Y24" s="9"/>
       <c r="Z24" s="9"/>
       <c r="AA24" s="9"/>
@@ -8936,75 +9131,73 @@
         <v>1</v>
       </c>
       <c r="B25" s="6"/>
-      <c r="C25" s="14">
-        <v>0</v>
-      </c>
-      <c r="D25" s="15">
-        <v>0</v>
-      </c>
-      <c r="E25" s="15">
-        <v>0</v>
-      </c>
-      <c r="F25" s="15">
-        <v>0</v>
-      </c>
-      <c r="G25" s="15">
-        <v>0</v>
-      </c>
-      <c r="H25" s="15">
-        <v>0</v>
-      </c>
-      <c r="I25" s="15">
-        <v>0</v>
-      </c>
-      <c r="J25" s="15">
-        <v>0</v>
-      </c>
-      <c r="K25" s="15">
-        <v>0</v>
-      </c>
-      <c r="L25" s="15">
+      <c r="C25" s="12">
+        <v>0</v>
+      </c>
+      <c r="D25" s="13">
+        <v>0</v>
+      </c>
+      <c r="E25" s="13">
+        <v>0</v>
+      </c>
+      <c r="F25" s="13">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0</v>
+      </c>
+      <c r="H25" s="13">
+        <v>0</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0</v>
+      </c>
+      <c r="J25" s="13">
+        <v>0</v>
+      </c>
+      <c r="K25" s="13">
+        <v>0</v>
+      </c>
+      <c r="L25" s="13">
         <v>6</v>
       </c>
-      <c r="M25" s="15">
+      <c r="M25" s="13">
         <v>41</v>
       </c>
-      <c r="N25" s="15">
+      <c r="N25" s="13">
         <v>399</v>
       </c>
-      <c r="O25" s="15">
-        <v>1864</v>
-      </c>
-      <c r="P25" s="15">
-        <v>5157</v>
-      </c>
-      <c r="Q25" s="11">
-        <v>8185</v>
-      </c>
-      <c r="R25" s="11">
-        <v>8248</v>
-      </c>
-      <c r="S25" s="11">
-        <v>6885</v>
-      </c>
-      <c r="T25" s="11">
-        <v>5151</v>
-      </c>
-      <c r="U25" s="11">
-        <v>3918</v>
-      </c>
-      <c r="V25" s="11">
-        <v>2806</v>
-      </c>
-      <c r="W25" s="11">
-        <v>2227</v>
-      </c>
-      <c r="X25" s="11">
-        <v>1728</v>
-      </c>
-      <c r="Y25" s="11">
-        <v>1205</v>
-      </c>
+      <c r="O25" s="13">
+        <v>1861</v>
+      </c>
+      <c r="P25" s="13">
+        <v>5149</v>
+      </c>
+      <c r="Q25" s="9">
+        <v>8172</v>
+      </c>
+      <c r="R25" s="9">
+        <v>8239</v>
+      </c>
+      <c r="S25" s="9">
+        <v>6870</v>
+      </c>
+      <c r="T25" s="9">
+        <v>5139</v>
+      </c>
+      <c r="U25" s="9">
+        <v>3911</v>
+      </c>
+      <c r="V25" s="9">
+        <v>2801</v>
+      </c>
+      <c r="W25" s="9">
+        <v>2206</v>
+      </c>
+      <c r="X25" s="9">
+        <v>1627</v>
+      </c>
+      <c r="Y25" s="9"/>
       <c r="Z25" s="9"/>
       <c r="AA25" s="9"/>
       <c r="AB25" s="9"/>
@@ -9081,78 +9274,76 @@
         <v>1</v>
       </c>
       <c r="B26" s="6"/>
-      <c r="C26" s="12">
-        <v>0</v>
-      </c>
-      <c r="D26" s="13">
-        <v>0</v>
-      </c>
-      <c r="E26" s="13">
-        <v>0</v>
-      </c>
-      <c r="F26" s="13">
-        <v>0</v>
-      </c>
-      <c r="G26" s="13">
-        <v>0</v>
-      </c>
-      <c r="H26" s="13">
-        <v>0</v>
-      </c>
-      <c r="I26" s="13">
-        <v>0</v>
-      </c>
-      <c r="J26" s="13">
-        <v>0</v>
-      </c>
-      <c r="K26" s="13">
-        <v>0</v>
-      </c>
-      <c r="L26" s="13">
+      <c r="C26" s="14">
+        <v>0</v>
+      </c>
+      <c r="D26" s="15">
+        <v>0</v>
+      </c>
+      <c r="E26" s="15">
+        <v>0</v>
+      </c>
+      <c r="F26" s="15">
+        <v>0</v>
+      </c>
+      <c r="G26" s="15">
+        <v>0</v>
+      </c>
+      <c r="H26" s="15">
+        <v>0</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0</v>
+      </c>
+      <c r="J26" s="15">
+        <v>0</v>
+      </c>
+      <c r="K26" s="15">
+        <v>0</v>
+      </c>
+      <c r="L26" s="15">
         <v>6</v>
       </c>
-      <c r="M26" s="13">
+      <c r="M26" s="15">
         <v>41</v>
       </c>
-      <c r="N26" s="13">
-        <v>401</v>
-      </c>
-      <c r="O26" s="13">
-        <v>1867</v>
-      </c>
-      <c r="P26" s="13">
-        <v>5165</v>
-      </c>
-      <c r="Q26" s="9">
-        <v>8192</v>
-      </c>
-      <c r="R26" s="9">
-        <v>8262</v>
-      </c>
-      <c r="S26" s="9">
-        <v>6895</v>
-      </c>
-      <c r="T26" s="9">
-        <v>5163</v>
-      </c>
-      <c r="U26" s="9">
-        <v>3935</v>
-      </c>
-      <c r="V26" s="9">
-        <v>2823</v>
-      </c>
-      <c r="W26" s="9">
-        <v>2231</v>
-      </c>
-      <c r="X26" s="9">
-        <v>1744</v>
-      </c>
-      <c r="Y26" s="9">
-        <v>1276</v>
-      </c>
-      <c r="Z26" s="9">
-        <v>865</v>
-      </c>
+      <c r="N26" s="15">
+        <v>399</v>
+      </c>
+      <c r="O26" s="15">
+        <v>1864</v>
+      </c>
+      <c r="P26" s="15">
+        <v>5157</v>
+      </c>
+      <c r="Q26" s="11">
+        <v>8185</v>
+      </c>
+      <c r="R26" s="11">
+        <v>8248</v>
+      </c>
+      <c r="S26" s="11">
+        <v>6885</v>
+      </c>
+      <c r="T26" s="11">
+        <v>5151</v>
+      </c>
+      <c r="U26" s="11">
+        <v>3918</v>
+      </c>
+      <c r="V26" s="11">
+        <v>2806</v>
+      </c>
+      <c r="W26" s="11">
+        <v>2227</v>
+      </c>
+      <c r="X26" s="11">
+        <v>1728</v>
+      </c>
+      <c r="Y26" s="11">
+        <v>1205</v>
+      </c>
+      <c r="Z26" s="9"/>
       <c r="AA26" s="9"/>
       <c r="AB26" s="9"/>
       <c r="AC26" s="9"/>
@@ -9265,44 +9456,42 @@
         <v>401</v>
       </c>
       <c r="O27" s="13">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="P27" s="13">
-        <v>5166</v>
+        <v>5165</v>
       </c>
       <c r="Q27" s="9">
-        <v>8197</v>
+        <v>8192</v>
       </c>
       <c r="R27" s="9">
-        <v>8269</v>
+        <v>8262</v>
       </c>
       <c r="S27" s="9">
-        <v>6899</v>
+        <v>6895</v>
       </c>
       <c r="T27" s="9">
-        <v>5170</v>
+        <v>5163</v>
       </c>
       <c r="U27" s="9">
-        <v>3947</v>
+        <v>3935</v>
       </c>
       <c r="V27" s="9">
-        <v>2838</v>
+        <v>2823</v>
       </c>
       <c r="W27" s="9">
-        <v>2244</v>
+        <v>2231</v>
       </c>
       <c r="X27" s="9">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="Y27" s="9">
-        <v>1279</v>
+        <v>1276</v>
       </c>
       <c r="Z27" s="9">
-        <v>915</v>
-      </c>
-      <c r="AA27" s="9">
-        <v>623</v>
-      </c>
+        <v>865</v>
+      </c>
+      <c r="AA27" s="9"/>
       <c r="AB27" s="9"/>
       <c r="AC27" s="9"/>
       <c r="AD27" s="9"/>
@@ -9372,6 +9561,155 @@
       <c r="CP27" s="9"/>
       <c r="CQ27" s="9"/>
     </row>
+    <row r="28" spans="1:96" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="12">
+        <v>0</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0</v>
+      </c>
+      <c r="F28" s="13">
+        <v>0</v>
+      </c>
+      <c r="G28" s="13">
+        <v>0</v>
+      </c>
+      <c r="H28" s="13">
+        <v>0</v>
+      </c>
+      <c r="I28" s="13">
+        <v>0</v>
+      </c>
+      <c r="J28" s="13">
+        <v>0</v>
+      </c>
+      <c r="K28" s="13">
+        <v>0</v>
+      </c>
+      <c r="L28" s="13">
+        <v>6</v>
+      </c>
+      <c r="M28" s="13">
+        <v>41</v>
+      </c>
+      <c r="N28" s="13">
+        <v>401</v>
+      </c>
+      <c r="O28" s="13">
+        <v>1868</v>
+      </c>
+      <c r="P28" s="13">
+        <v>5166</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>8197</v>
+      </c>
+      <c r="R28" s="9">
+        <v>8269</v>
+      </c>
+      <c r="S28" s="9">
+        <v>6899</v>
+      </c>
+      <c r="T28" s="9">
+        <v>5170</v>
+      </c>
+      <c r="U28" s="9">
+        <v>3947</v>
+      </c>
+      <c r="V28" s="9">
+        <v>2838</v>
+      </c>
+      <c r="W28" s="9">
+        <v>2244</v>
+      </c>
+      <c r="X28" s="9">
+        <v>1747</v>
+      </c>
+      <c r="Y28" s="9">
+        <v>1279</v>
+      </c>
+      <c r="Z28" s="9">
+        <v>915</v>
+      </c>
+      <c r="AA28" s="9">
+        <v>623</v>
+      </c>
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="9"/>
+      <c r="AG28" s="9"/>
+      <c r="AH28" s="9"/>
+      <c r="AI28" s="9"/>
+      <c r="AJ28" s="9"/>
+      <c r="AK28" s="9"/>
+      <c r="AL28" s="9"/>
+      <c r="AM28" s="9"/>
+      <c r="AN28" s="9"/>
+      <c r="AO28" s="9"/>
+      <c r="AP28" s="9"/>
+      <c r="AQ28" s="9"/>
+      <c r="AR28" s="9"/>
+      <c r="AS28" s="9"/>
+      <c r="AT28" s="9"/>
+      <c r="AU28" s="9"/>
+      <c r="AV28" s="9"/>
+      <c r="AW28" s="9"/>
+      <c r="AX28" s="9"/>
+      <c r="AY28" s="9"/>
+      <c r="AZ28" s="9"/>
+      <c r="BA28" s="9"/>
+      <c r="BB28" s="9"/>
+      <c r="BC28" s="9"/>
+      <c r="BD28" s="9"/>
+      <c r="BE28" s="9"/>
+      <c r="BF28" s="9"/>
+      <c r="BG28" s="9"/>
+      <c r="BH28" s="9"/>
+      <c r="BI28" s="9"/>
+      <c r="BJ28" s="9"/>
+      <c r="BK28" s="9"/>
+      <c r="BL28" s="9"/>
+      <c r="BM28" s="9"/>
+      <c r="BN28" s="9"/>
+      <c r="BO28" s="9"/>
+      <c r="BP28" s="9"/>
+      <c r="BQ28" s="9"/>
+      <c r="BR28" s="9"/>
+      <c r="BS28" s="9"/>
+      <c r="BT28" s="9"/>
+      <c r="BU28" s="9"/>
+      <c r="BV28" s="9"/>
+      <c r="BW28" s="9"/>
+      <c r="BX28" s="9"/>
+      <c r="BY28" s="9"/>
+      <c r="BZ28" s="9"/>
+      <c r="CA28" s="9"/>
+      <c r="CB28" s="9"/>
+      <c r="CC28" s="9"/>
+      <c r="CD28" s="9"/>
+      <c r="CE28" s="9"/>
+      <c r="CF28" s="9"/>
+      <c r="CG28" s="9"/>
+      <c r="CH28" s="9"/>
+      <c r="CI28" s="9"/>
+      <c r="CJ28" s="9"/>
+      <c r="CK28" s="9"/>
+      <c r="CL28" s="9"/>
+      <c r="CM28" s="9"/>
+      <c r="CN28" s="9"/>
+      <c r="CO28" s="9"/>
+      <c r="CP28" s="9"/>
+      <c r="CQ28" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9382,7 +9720,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>